<commit_message>
Updated bom and adjusted connector position
</commit_message>
<xml_diff>
--- a/PCB/Lixie_II_Reverse_LED_BOM.xlsx
+++ b/PCB/Lixie_II_Reverse_LED_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dustin\Documents\Personal\GIT\LIXIE\Lixie_II_OSHW\HARDWARE\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwestaby\Documents\Personal\GIT\LIXIE\Lixie_II_OSHW\HARDWARE\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FBC3D830-04DC-4CA5-874E-3C9C777ECB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A994DB-6CFF-4DE1-9194-FCE54B940E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17025"/>
+    <workbookView xWindow="34170" yWindow="3240" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -46,15 +46,9 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C0402</t>
-  </si>
-  <si>
     <t>Capacitor</t>
   </si>
   <si>
-    <t>C52923</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -221,12 +215,18 @@
   </si>
   <si>
     <t>1x3</t>
+  </si>
+  <si>
+    <t>C15849</t>
+  </si>
+  <si>
+    <t>C0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -571,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -606,16 +606,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -623,16 +623,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -640,16 +640,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -657,16 +657,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -674,16 +674,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -691,16 +691,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -725,16 +725,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -742,16 +742,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -759,16 +759,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -776,16 +776,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -793,16 +793,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -810,16 +810,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -827,16 +827,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -861,16 +861,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -878,16 +878,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -895,16 +895,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -912,16 +912,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -929,16 +929,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
@@ -946,16 +946,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -963,16 +963,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -980,372 +980,372 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
         <v>58</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
       <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
         <v>60</v>
       </c>
-      <c r="D25" t="s">
-        <v>62</v>
-      </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
         <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>